<commit_message>
Commit para actualizarlo todo
Este commit se hace para volcar todo lo que hay en dropbox una vez
ordenado y de esta forma llevar todo el control de versionado
</commit_message>
<xml_diff>
--- a/1º Iteración/Grupo Planificación y Gestión/Carga de trabajo v2.xlsx
+++ b/1º Iteración/Grupo Planificación y Gestión/Carga de trabajo v2.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="15480" windowHeight="8025"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="15480" windowHeight="8025" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Análisis" sheetId="1" r:id="rId1"/>
     <sheet name="Implementacion" sheetId="2" r:id="rId2"/>
-    <sheet name="Gestion" sheetId="3" r:id="rId3"/>
+    <sheet name="Planificacion" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="76">
   <si>
     <t>Diagrama CU</t>
   </si>
@@ -106,32 +106,6 @@
   </si>
   <si>
     <t>Diag Clases Diseño (cont)</t>
-  </si>
-  <si>
-    <r>
-      <t>Diagrama secuencia "</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Sistema</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"</t>
-    </r>
   </si>
   <si>
     <r>
@@ -186,9 +160,6 @@
     </r>
   </si>
   <si>
-    <t>Diag. Componentes</t>
-  </si>
-  <si>
     <t>Corrección de errores dichos por el grupo de implementación</t>
   </si>
   <si>
@@ -250,9 +221,6 @@
   </si>
   <si>
     <t xml:space="preserve">Contratos </t>
-  </si>
-  <si>
-    <t>Acabar Trabajo Atrasado</t>
   </si>
   <si>
     <t>Sabado 17</t>
@@ -292,12 +260,93 @@
   <si>
     <t>Crear BD</t>
   </si>
+  <si>
+    <t>Antonio Rodriguez</t>
+  </si>
+  <si>
+    <t>Raul Lopez</t>
+  </si>
+  <si>
+    <t>Juan Antonio</t>
+  </si>
+  <si>
+    <t>Alberto Bailon</t>
+  </si>
+  <si>
+    <t>Lunes 5</t>
+  </si>
+  <si>
+    <t>Martes 6</t>
+  </si>
+  <si>
+    <t>Diagrama de Gantt</t>
+  </si>
+  <si>
+    <t>Documento de planificacion</t>
+  </si>
+  <si>
+    <t>Entrega de planificacion</t>
+  </si>
+  <si>
+    <t>Pruebas en programa</t>
+  </si>
+  <si>
+    <t>Recursos del proyecto</t>
+  </si>
+  <si>
+    <t>Revision de planificación</t>
+  </si>
+  <si>
+    <t>Diagrama de Pert</t>
+  </si>
+  <si>
+    <t>Retrasos de trabajo</t>
+  </si>
+  <si>
+    <t>Fallo familiares</t>
+  </si>
+  <si>
+    <t>Faltaban tareas</t>
+  </si>
+  <si>
+    <t>Diag.Secuencia "Objetos"</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Diagrama secuencia "</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sistema</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -359,8 +408,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -403,8 +480,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="24">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -425,55 +508,6 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -665,11 +699,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -677,47 +735,47 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -739,40 +797,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -781,20 +852,17 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1099,21 +1167,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="H3" activeCellId="1" sqref="F3 H3"/>
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.28515625" customWidth="1"/>
-    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.140625" customWidth="1"/>
-    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.7109375" customWidth="1"/>
-    <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
+    <col min="5" max="5" width="5.42578125" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" customWidth="1"/>
+    <col min="7" max="7" width="5.42578125" customWidth="1"/>
+    <col min="8" max="8" width="27.140625" customWidth="1"/>
+    <col min="9" max="9" width="5.42578125" customWidth="1"/>
     <col min="11" max="11" width="18.42578125" customWidth="1"/>
     <col min="12" max="12" width="23.140625" customWidth="1"/>
   </cols>
@@ -1152,13 +1220,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
@@ -1258,13 +1326,13 @@
         <v>7</v>
       </c>
       <c r="B6" s="41" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
       </c>
       <c r="D6" s="42" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E6" s="2">
         <v>2</v>
@@ -1287,13 +1355,13 @@
         <v>8</v>
       </c>
       <c r="B7" s="41" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>30</v>
+      <c r="D7" s="42" t="s">
+        <v>56</v>
       </c>
       <c r="E7" s="2">
         <v>2</v>
@@ -1315,55 +1383,39 @@
       <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="1">
-        <v>2</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="2">
-        <v>2</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="3">
-        <v>2</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I8" s="4">
-        <v>2</v>
-      </c>
+      <c r="B8" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="41">
+        <v>2</v>
+      </c>
+      <c r="D8" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="42">
+        <v>2</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="39" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" s="1">
-        <v>2</v>
-      </c>
-      <c r="D9" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" s="2">
-        <v>2</v>
-      </c>
+      <c r="B9" s="39"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="2"/>
       <c r="F9" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G9" s="3">
         <v>2</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I9" s="4">
         <v>2</v>
@@ -1377,7 +1429,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C10" s="1">
         <v>2</v>
@@ -1389,13 +1441,13 @@
         <v>2</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G10" s="3">
         <v>2</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I10" s="4">
         <v>2</v>
@@ -1406,32 +1458,24 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C11" s="1">
         <v>2</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E11" s="2">
         <v>2</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G11" s="3">
-        <v>2</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I11" s="4">
-        <v>2</v>
-      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
@@ -1439,70 +1483,124 @@
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="2" t="s">
-        <v>33</v>
+      <c r="D12" s="59" t="s">
+        <v>75</v>
       </c>
       <c r="E12" s="2">
         <v>2</v>
       </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
+      <c r="F12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="3">
+        <v>2</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="49" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="50"/>
-      <c r="H13" s="50"/>
-      <c r="I13" s="51"/>
+      <c r="B13" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="15">
+        <v>2</v>
+      </c>
+      <c r="D13" s="59" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="2">
+        <v>2</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="3">
+        <v>2</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="52"/>
-      <c r="C14" s="53"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="53"/>
-      <c r="H14" s="53"/>
-      <c r="I14" s="54"/>
+      <c r="B14" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="15">
+        <v>2</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" s="27">
+        <v>2</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="3">
+        <v>2</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I14" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="52"/>
-      <c r="C15" s="53"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="53"/>
-      <c r="F15" s="53"/>
-      <c r="G15" s="53"/>
-      <c r="H15" s="53"/>
-      <c r="I15" s="54"/>
+      <c r="B15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="2">
+        <v>2</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="3">
+        <v>2</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I15" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="55"/>
-      <c r="C16" s="56"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="56"/>
-      <c r="H16" s="56"/>
-      <c r="I16" s="57"/>
+      <c r="B16" s="71"/>
+      <c r="C16" s="72"/>
+      <c r="D16" s="72"/>
+      <c r="E16" s="72"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
     </row>
     <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
@@ -1517,100 +1615,99 @@
     </row>
     <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="58" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="58"/>
-      <c r="D18" s="58"/>
-      <c r="E18" s="58"/>
-      <c r="F18" s="58"/>
-      <c r="G18" s="58"/>
-      <c r="H18" s="58"/>
-      <c r="I18" s="58"/>
+        <v>36</v>
+      </c>
+      <c r="B18" s="73" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="73"/>
+      <c r="D18" s="73"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="73"/>
+      <c r="G18" s="73"/>
+      <c r="H18" s="73"/>
+      <c r="I18" s="73"/>
     </row>
     <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="58"/>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="58"/>
-      <c r="F19" s="58"/>
-      <c r="G19" s="58"/>
-      <c r="H19" s="58"/>
-      <c r="I19" s="58"/>
+        <v>37</v>
+      </c>
+      <c r="B19" s="73"/>
+      <c r="C19" s="73"/>
+      <c r="D19" s="73"/>
+      <c r="E19" s="73"/>
+      <c r="F19" s="73"/>
+      <c r="G19" s="73"/>
+      <c r="H19" s="73"/>
+      <c r="I19" s="73"/>
     </row>
     <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="58"/>
-      <c r="C20" s="58"/>
-      <c r="D20" s="58"/>
-      <c r="E20" s="58"/>
-      <c r="F20" s="58"/>
-      <c r="G20" s="58"/>
-      <c r="H20" s="58"/>
-      <c r="I20" s="58"/>
+        <v>38</v>
+      </c>
+      <c r="B20" s="73"/>
+      <c r="C20" s="73"/>
+      <c r="D20" s="73"/>
+      <c r="E20" s="73"/>
+      <c r="F20" s="73"/>
+      <c r="G20" s="73"/>
+      <c r="H20" s="73"/>
+      <c r="I20" s="73"/>
     </row>
     <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" s="58"/>
-      <c r="C21" s="58"/>
-      <c r="D21" s="58"/>
-      <c r="E21" s="58"/>
-      <c r="F21" s="58"/>
-      <c r="G21" s="58"/>
-      <c r="H21" s="58"/>
-      <c r="I21" s="58"/>
+        <v>39</v>
+      </c>
+      <c r="B21" s="73"/>
+      <c r="C21" s="73"/>
+      <c r="D21" s="73"/>
+      <c r="E21" s="73"/>
+      <c r="F21" s="73"/>
+      <c r="G21" s="73"/>
+      <c r="H21" s="73"/>
+      <c r="I21" s="73"/>
     </row>
     <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="58"/>
-      <c r="C22" s="58"/>
-      <c r="D22" s="58"/>
-      <c r="E22" s="58"/>
-      <c r="F22" s="58"/>
-      <c r="G22" s="58"/>
-      <c r="H22" s="58"/>
-      <c r="I22" s="58"/>
+        <v>40</v>
+      </c>
+      <c r="B22" s="73"/>
+      <c r="C22" s="73"/>
+      <c r="D22" s="73"/>
+      <c r="E22" s="73"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="73"/>
+      <c r="H22" s="73"/>
+      <c r="I22" s="73"/>
     </row>
     <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="22"/>
       <c r="C23" s="22">
         <f>SUM(C2:C22)</f>
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D23" s="22"/>
       <c r="E23" s="22">
         <f t="shared" ref="E23" si="0">SUM(E2:E22)</f>
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F23" s="22"/>
       <c r="G23" s="22">
         <f t="shared" ref="G23" si="1">SUM(G2:G22)</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="H23" s="22"/>
       <c r="I23" s="22">
         <f t="shared" ref="I23" si="2">SUM(I2:I22)</f>
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B13:I16"/>
+  <mergeCells count="1">
     <mergeCell ref="B18:I22"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
@@ -1619,8 +1716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1640,25 +1737,25 @@
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5"/>
       <c r="B1" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>1</v>
@@ -1668,92 +1765,92 @@
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="59" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
+      <c r="B2" s="74" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="76"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="62"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="64"/>
+      <c r="B3" s="77"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="79"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="62"/>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="63"/>
-      <c r="H4" s="63"/>
-      <c r="I4" s="64"/>
+      <c r="B4" s="77"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="79"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
-      <c r="B5" s="62"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="63"/>
-      <c r="H5" s="63"/>
-      <c r="I5" s="64"/>
+      <c r="B5" s="77"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="78"/>
+      <c r="H5" s="78"/>
+      <c r="I5" s="79"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="62"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="63"/>
-      <c r="H6" s="63"/>
-      <c r="I6" s="64"/>
+      <c r="B6" s="77"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="78"/>
+      <c r="E6" s="78"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="78"/>
+      <c r="H6" s="78"/>
+      <c r="I6" s="79"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="62"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="63"/>
-      <c r="H7" s="63"/>
-      <c r="I7" s="64"/>
+      <c r="B7" s="77"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78"/>
+      <c r="F7" s="78"/>
+      <c r="G7" s="78"/>
+      <c r="H7" s="78"/>
+      <c r="I7" s="79"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="65"/>
-      <c r="C8" s="66"/>
-      <c r="D8" s="66"/>
-      <c r="E8" s="66"/>
-      <c r="F8" s="66"/>
-      <c r="G8" s="66"/>
-      <c r="H8" s="66"/>
-      <c r="I8" s="67"/>
+      <c r="B8" s="80"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="81"/>
+      <c r="G8" s="81"/>
+      <c r="H8" s="81"/>
+      <c r="I8" s="82"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
@@ -1774,25 +1871,25 @@
         <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C10" s="1">
         <v>2</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E10" s="2">
         <v>2</v>
       </c>
       <c r="F10" s="47" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G10" s="47">
         <v>2</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I10" s="4">
         <v>2</v>
@@ -1801,28 +1898,28 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C11" s="1">
         <v>2</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E11" s="2">
         <v>2</v>
       </c>
       <c r="F11" s="47" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G11" s="47">
         <v>2</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I11" s="4">
         <v>2</v>
@@ -1845,25 +1942,25 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C13" s="1">
         <v>2</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E13" s="2">
         <v>2</v>
       </c>
       <c r="F13" s="47" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G13" s="47">
         <v>2</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I13" s="4">
         <v>1</v>
@@ -1874,25 +1971,25 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2</v>
+      </c>
+      <c r="D14" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="48">
+        <v>2</v>
+      </c>
+      <c r="F14" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="47">
+        <v>2</v>
+      </c>
+      <c r="H14" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="C14" s="1">
-        <v>2</v>
-      </c>
-      <c r="D14" s="48" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="48">
-        <v>2</v>
-      </c>
-      <c r="F14" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="G14" s="47">
-        <v>2</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>45</v>
       </c>
       <c r="I14" s="4">
         <v>2</v>
@@ -1903,25 +2000,25 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="15">
+        <v>2</v>
+      </c>
+      <c r="D15" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="26">
+        <v>2</v>
+      </c>
+      <c r="F15" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="19">
+        <v>2</v>
+      </c>
+      <c r="H15" s="30" t="s">
         <v>43</v>
-      </c>
-      <c r="C15" s="15">
-        <v>2</v>
-      </c>
-      <c r="D15" s="48" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="26">
-        <v>2</v>
-      </c>
-      <c r="F15" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="G15" s="19">
-        <v>2</v>
-      </c>
-      <c r="H15" s="30" t="s">
-        <v>45</v>
       </c>
       <c r="I15" s="30">
         <v>2</v>
@@ -1932,25 +2029,25 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="15">
+        <v>2</v>
+      </c>
+      <c r="D16" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="26">
+        <v>2</v>
+      </c>
+      <c r="F16" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" s="19">
+        <v>2</v>
+      </c>
+      <c r="H16" s="30" t="s">
         <v>43</v>
-      </c>
-      <c r="C16" s="15">
-        <v>2</v>
-      </c>
-      <c r="D16" s="48" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" s="26">
-        <v>2</v>
-      </c>
-      <c r="F16" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="G16" s="19">
-        <v>2</v>
-      </c>
-      <c r="H16" s="30" t="s">
-        <v>45</v>
       </c>
       <c r="I16" s="30">
         <v>2</v>
@@ -1982,70 +2079,70 @@
     </row>
     <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="58" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="58"/>
-      <c r="F19" s="58"/>
-      <c r="G19" s="58"/>
-      <c r="H19" s="58"/>
-      <c r="I19" s="58"/>
+        <v>36</v>
+      </c>
+      <c r="B19" s="73" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="73"/>
+      <c r="D19" s="73"/>
+      <c r="E19" s="73"/>
+      <c r="F19" s="73"/>
+      <c r="G19" s="73"/>
+      <c r="H19" s="73"/>
+      <c r="I19" s="73"/>
     </row>
     <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="58"/>
-      <c r="C20" s="58"/>
-      <c r="D20" s="58"/>
-      <c r="E20" s="58"/>
-      <c r="F20" s="58"/>
-      <c r="G20" s="58"/>
-      <c r="H20" s="58"/>
-      <c r="I20" s="58"/>
+        <v>37</v>
+      </c>
+      <c r="B20" s="73"/>
+      <c r="C20" s="73"/>
+      <c r="D20" s="73"/>
+      <c r="E20" s="73"/>
+      <c r="F20" s="73"/>
+      <c r="G20" s="73"/>
+      <c r="H20" s="73"/>
+      <c r="I20" s="73"/>
     </row>
     <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="58"/>
-      <c r="C21" s="58"/>
-      <c r="D21" s="58"/>
-      <c r="E21" s="58"/>
-      <c r="F21" s="58"/>
-      <c r="G21" s="58"/>
-      <c r="H21" s="58"/>
-      <c r="I21" s="58"/>
+        <v>38</v>
+      </c>
+      <c r="B21" s="73"/>
+      <c r="C21" s="73"/>
+      <c r="D21" s="73"/>
+      <c r="E21" s="73"/>
+      <c r="F21" s="73"/>
+      <c r="G21" s="73"/>
+      <c r="H21" s="73"/>
+      <c r="I21" s="73"/>
     </row>
     <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="58"/>
-      <c r="C22" s="58"/>
-      <c r="D22" s="58"/>
-      <c r="E22" s="58"/>
-      <c r="F22" s="58"/>
-      <c r="G22" s="58"/>
-      <c r="H22" s="58"/>
-      <c r="I22" s="58"/>
+        <v>39</v>
+      </c>
+      <c r="B22" s="73"/>
+      <c r="C22" s="73"/>
+      <c r="D22" s="73"/>
+      <c r="E22" s="73"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="73"/>
+      <c r="H22" s="73"/>
+      <c r="I22" s="73"/>
     </row>
     <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="58"/>
-      <c r="C23" s="58"/>
-      <c r="D23" s="58"/>
-      <c r="E23" s="58"/>
-      <c r="F23" s="58"/>
-      <c r="G23" s="58"/>
-      <c r="H23" s="58"/>
-      <c r="I23" s="58"/>
+        <v>40</v>
+      </c>
+      <c r="B23" s="73"/>
+      <c r="C23" s="73"/>
+      <c r="D23" s="73"/>
+      <c r="E23" s="73"/>
+      <c r="F23" s="73"/>
+      <c r="G23" s="73"/>
+      <c r="H23" s="73"/>
+      <c r="I23" s="73"/>
     </row>
     <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="22"/>
@@ -2081,12 +2178,434 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" customWidth="1"/>
+    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25" customWidth="1"/>
+    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.28515625" customWidth="1"/>
+    <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.85546875" customWidth="1"/>
+    <col min="11" max="11" width="21.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="5"/>
+      <c r="B1" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="51" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="52" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="52" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="58" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="58">
+        <v>2</v>
+      </c>
+      <c r="D2" s="70" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="59">
+        <v>2</v>
+      </c>
+      <c r="F2" s="60" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" s="60">
+        <v>1</v>
+      </c>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="53" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="58" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="58">
+        <v>2</v>
+      </c>
+      <c r="D3" s="59" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="59">
+        <v>2</v>
+      </c>
+      <c r="F3" s="60" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" s="60">
+        <v>1</v>
+      </c>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="58"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="61"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="53" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="61"/>
+      <c r="J5" t="s">
+        <v>69</v>
+      </c>
+      <c r="K5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="58"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="61"/>
+      <c r="I6" s="61"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="54"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="62"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="53" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="58"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="60"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="61"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="58"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="61"/>
+      <c r="I9" s="61"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="83" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="84"/>
+      <c r="D10" s="84"/>
+      <c r="E10" s="84"/>
+      <c r="F10" s="84"/>
+      <c r="G10" s="84"/>
+      <c r="H10" s="84"/>
+      <c r="I10" s="85"/>
+      <c r="J10" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="53" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="63"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="60" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" s="60">
+        <v>2</v>
+      </c>
+      <c r="H11" s="61"/>
+      <c r="I11" s="61"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="58"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="61"/>
+      <c r="I12" s="61"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="58"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="60"/>
+      <c r="H13" s="61"/>
+      <c r="I13" s="61"/>
+      <c r="J13" t="s">
+        <v>69</v>
+      </c>
+      <c r="K13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="55"/>
+      <c r="B14" s="65"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="65"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="53" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="58"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="60"/>
+      <c r="H15" s="61"/>
+      <c r="I15" s="61"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="53" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="58"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="59"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="61"/>
+      <c r="I16" s="61"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="53" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="58"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="60"/>
+      <c r="H17" s="61"/>
+      <c r="I17" s="61"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="58"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="61"/>
+      <c r="I18" s="61"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="66"/>
+      <c r="C19" s="66"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="67"/>
+      <c r="F19" s="68"/>
+      <c r="G19" s="68"/>
+      <c r="H19" s="69"/>
+      <c r="I19" s="69"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="53"/>
+      <c r="B20" s="65"/>
+      <c r="C20" s="65"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="65"/>
+      <c r="F20" s="65"/>
+      <c r="G20" s="65"/>
+      <c r="H20" s="65"/>
+      <c r="I20" s="65"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="57" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="83" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="84"/>
+      <c r="D21" s="84"/>
+      <c r="E21" s="84"/>
+      <c r="F21" s="84"/>
+      <c r="G21" s="84"/>
+      <c r="H21" s="84"/>
+      <c r="I21" s="85"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="57" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="58"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="60"/>
+      <c r="G22" s="60"/>
+      <c r="H22" s="61"/>
+      <c r="I22" s="61"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="57" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="58"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="59"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="60"/>
+      <c r="H23" s="61"/>
+      <c r="I23" s="61"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="57" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="58"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="59"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="60"/>
+      <c r="G24" s="60"/>
+      <c r="H24" s="61"/>
+      <c r="I24" s="61"/>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="57" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="58"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="60"/>
+      <c r="G25" s="60"/>
+      <c r="H25" s="61"/>
+      <c r="I25" s="61"/>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="22">
+        <f>SUM(C2:C25)</f>
+        <v>4</v>
+      </c>
+      <c r="E26" s="22">
+        <f>SUM(E2:E25)</f>
+        <v>4</v>
+      </c>
+      <c r="G26" s="22">
+        <f>SUM(G2:G25)</f>
+        <v>4</v>
+      </c>
+      <c r="I26" s="22">
+        <f>SUM(I4:I25)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="B21:I21"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>